<commit_message>
Actualizacion clase reportes en PDF
</commit_message>
<xml_diff>
--- a/ReportesExcel/resultadoPcfactory.xlsx
+++ b/ReportesExcel/resultadoPcfactory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
   <si>
     <t>Id_Producto</t>
   </si>
@@ -402,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -537,6 +537,186 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>